<commit_message>
Changes: -combined all database controllers into one file -began work on the user verification engine -changed the layout of the users_logged_in.json -removed the "Database Name" Property from dbinfo -added a dbname parameter to all functions requiring a db name -added a JsonProp.py to the JSON Data dir. -NOTE: JsonProp will be used to house all json props used in all files -Updated the readme Document to explain what each file does
</commit_message>
<xml_diff>
--- a/Readme Files/Expected Table Layout as a Spreadsheet.xlsx
+++ b/Readme Files/Expected Table Layout as a Spreadsheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aseefried/GitHub/GameTrackerUltimate/Readme Files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD571D-1A3E-9148-979F-787FD997D1B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16245" yWindow="1545" windowWidth="38355" windowHeight="13110" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
   <si>
     <t>Drive name</t>
   </si>
@@ -170,13 +176,28 @@
   </si>
   <si>
     <t>access lev</t>
+  </si>
+  <si>
+    <t>Number of Games</t>
+  </si>
+  <si>
+    <t>Favored publisher</t>
+  </si>
+  <si>
+    <t>Favored Genre</t>
+  </si>
+  <si>
+    <t>Favored Platform</t>
+  </si>
+  <si>
+    <t>Top game tag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +234,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -259,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,9 +320,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,6 +372,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,24 +565,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -563,7 +628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -586,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -615,25 +680,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -656,7 +721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -679,7 +744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -699,7 +764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -725,7 +790,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -745,7 +810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -765,7 +830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -785,7 +850,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -805,7 +870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -831,7 +896,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -851,7 +916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -871,7 +936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -891,7 +956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -911,7 +976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -931,7 +996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -951,7 +1016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -971,7 +1036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -991,7 +1056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -1011,7 +1076,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -1031,7 +1096,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>43</v>
       </c>
@@ -1051,7 +1116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>44</v>
       </c>
@@ -1071,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>45</v>
       </c>
@@ -1091,7 +1156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>46</v>
       </c>
@@ -1117,20 +1182,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1142,6 +1212,21 @@
       </c>
       <c r="D1" t="s">
         <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1150,12 +1235,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>